<commit_message>
Added D.Samuel back in to 49ers players data
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/Players Data.xlsx
+++ b/Base/Teams/49ers/Players Data.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Teams/49ers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_1558CAC74A91005605703837F5EA457781334ECB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A508EF98-FD0D-4F61-8724-49A4A77B6319}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rushing" sheetId="1" r:id="rId1"/>
     <sheet name="Receiving" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -90,13 +96,16 @@
   </si>
   <si>
     <t>C.Woerner</t>
+  </si>
+  <si>
+    <t>D.Samuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,13 +153,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -159,6 +182,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -205,7 +236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +268,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,6 +320,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,14 +513,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -490,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -510,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -530,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -550,7 +619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -570,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -590,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -610,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -630,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -650,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -668,6 +737,26 @@
       </c>
       <c r="F11">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -676,14 +765,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +797,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -732,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -758,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -784,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -810,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -836,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -862,7 +953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -888,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -914,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -940,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -966,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -992,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1016,6 +1107,32 @@
       </c>
       <c r="H13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>